<commit_message>
18/02/2026 - Reportes Actualizados, Acta de Validación PDF y Word actualizados, Acta de Cómputo Total PDF y Word agregados
</commit_message>
<xml_diff>
--- a/plantillas/Incidentes.xlsx
+++ b/plantillas/Incidentes.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D836A7B8-34CB-4B24-A711-8040514C8B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8529F3-DFD2-4EA7-856C-3AE94720DFD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Participantes</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Nombre de la Unidad Territorial</t>
-  </si>
-  <si>
-    <t>FORMATO 3</t>
   </si>
   <si>
     <t>Fecha:</t>
@@ -88,7 +85,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,20 +119,6 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -199,8 +182,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,38 +198,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC0C0C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -323,30 +291,21 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -354,80 +313,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -739,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH19"/>
+  <dimension ref="A1:AH20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1202,275 +1167,282 @@
     <col min="16146" max="16146" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
+    <row r="1" spans="1:34" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
     </row>
     <row r="2" spans="1:34" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
     </row>
     <row r="3" spans="1:34" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
-    </row>
-    <row r="4" spans="1:34" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-    </row>
-    <row r="5" spans="1:34" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="22"/>
-      <c r="Q5" s="22"/>
-      <c r="R5" s="22"/>
-    </row>
-    <row r="6" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="33" t="s">
+      <c r="A3" s="21"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+    </row>
+    <row r="4" spans="1:34" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+    </row>
+    <row r="5" spans="1:34" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+    </row>
+    <row r="6" spans="1:34" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="2"/>
+    </row>
+    <row r="7" spans="1:34" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="33"/>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="34"/>
+      <c r="R7" s="34"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="3"/>
+      <c r="AH7" s="3"/>
+    </row>
+    <row r="8" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="19"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="P6" s="4"/>
-    </row>
-    <row r="7" spans="1:34" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="29"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="28"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
-      <c r="U7" s="5"/>
-      <c r="V7" s="5"/>
-      <c r="W7" s="5"/>
-      <c r="X7" s="5"/>
-      <c r="Y7" s="5"/>
-      <c r="Z7" s="5"/>
-      <c r="AA7" s="5"/>
-      <c r="AB7" s="5"/>
-      <c r="AC7" s="5"/>
-      <c r="AD7" s="5"/>
-      <c r="AE7" s="5"/>
-      <c r="AF7" s="5"/>
-      <c r="AG7" s="5"/>
-      <c r="AH7" s="5"/>
-    </row>
-    <row r="8" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="3"/>
+      <c r="R8" s="6"/>
     </row>
     <row r="9" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="27"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="10" t="s">
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="N9" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="R9" s="9"/>
-    </row>
-    <row r="10" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P9" s="6"/>
+    </row>
+    <row r="10" spans="1:34" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G10" s="31"/>
       <c r="H10" s="31"/>
       <c r="I10" s="31"/>
       <c r="J10" s="31"/>
       <c r="K10" s="31"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="24" t="s">
+      <c r="L10" s="27"/>
+      <c r="P10" s="28"/>
+    </row>
+    <row r="11" spans="1:34" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="M11" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="N11" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="O11" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="P11" s="28"/>
+    </row>
+    <row r="12" spans="1:34" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="36"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="R10" s="9"/>
-    </row>
-    <row r="11" spans="1:34" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="26" t="s">
+      <c r="H12" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="26" t="s">
+      <c r="I12" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="26" t="s">
+      <c r="J12" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="J11" s="26" t="s">
+      <c r="K12" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="K11" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="L11" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="M11" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="N11" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="O11" s="25" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="L14" s="11"/>
-      <c r="M14" s="12"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="L15" s="13"/>
-      <c r="M15" s="14"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="9"/>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="L16" s="11"/>
-      <c r="M16" s="12"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="11"/>
     </row>
     <row r="17" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L17" s="13"/>
-      <c r="M17" s="14"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="9"/>
     </row>
     <row r="18" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L18" s="15"/>
-      <c r="M18" s="16"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="11"/>
     </row>
     <row r="19" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L19" s="15"/>
-      <c r="M19" s="16"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="13"/>
+    </row>
+    <row r="20" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L20" s="12"/>
+      <c r="M20" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.26" right="0.23" top="0.43" bottom="0.33" header="0.17" footer="0.17"/>

</xml_diff>